<commit_message>
excel feed-in 0 entfernt
</commit_message>
<xml_diff>
--- a/course_project/data/cum_and_ann_installed_cap_bundesland.xlsx
+++ b/course_project/data/cum_and_ann_installed_cap_bundesland.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andi Eckmann\Desktop\ETH Studium\MASTERSTUDIUM\2. Semester\Big Data for Public Policy\big_data_policy_2020\course_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6F71AD-1F14-4E6C-9BB6-AAE86AED4064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B396F31F-F4A2-4BCA-BCCC-5C735C0706C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:N501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F2:F10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,7 +502,7 @@
     <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="19.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.77734375" customWidth="1"/>
     <col min="9" max="9" width="11.77734375" customWidth="1"/>

</xml_diff>